<commit_message>
Nytt opsett for excel
</commit_message>
<xml_diff>
--- a/Load_Profile/ramp/input_files/Appliances_and_users.xlsx
+++ b/Load_Profile/ramp/input_files/Appliances_and_users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varsh\PycharmProjects\SizingOffGridMicrogrids\Load_Profile\ramp\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C0F5B74-3368-4FCE-B5F6-7012C171DDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E255F7A-B76E-429C-9B31-63E8478AAF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DD404E9A-0D1E-45D4-8190-461235976194}"/>
+    <workbookView xWindow="28680" yWindow="-6165" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{DD404E9A-0D1E-45D4-8190-461235976194}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" r:id="rId1"/>
@@ -40,71 +40,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>A</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>n_user</t>
-  </si>
-  <si>
-    <t>us-pref</t>
-  </si>
-  <si>
-    <t>Appliance</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>num-windows</t>
-  </si>
-  <si>
-    <t>func-time</t>
-  </si>
-  <si>
-    <t>r_t</t>
-  </si>
-  <si>
-    <t>func_cycle</t>
-  </si>
-  <si>
-    <t>fixed</t>
-  </si>
-  <si>
-    <t>fixed_cycle</t>
-  </si>
-  <si>
-    <t>occasional_use</t>
-  </si>
-  <si>
-    <t>flat</t>
-  </si>
-  <si>
-    <t>thermal_P_var</t>
-  </si>
-  <si>
-    <t>pref_index</t>
-  </si>
-  <si>
-    <t>wd_we_type</t>
-  </si>
-  <si>
-    <t>year_min</t>
-  </si>
-  <si>
-    <t>initial_share</t>
-  </si>
-  <si>
-    <t>Connected user</t>
-  </si>
-  <si>
     <t>Phone</t>
   </si>
   <si>
@@ -120,20 +60,71 @@
     <t>Fan</t>
   </si>
   <si>
-    <t>Start_time</t>
-  </si>
-  <si>
-    <t>End_time</t>
-  </si>
-  <si>
     <t>visitor_hut_1,visitor_hut_2</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>Number of Users</t>
+  </si>
+  <si>
+    <t>User Preference</t>
+  </si>
+  <si>
+    <t>Appliance Name</t>
+  </si>
+  <si>
+    <t>Power of Appliance</t>
+  </si>
+  <si>
+    <t>Number of Appliances</t>
+  </si>
+  <si>
+    <t>Number of Functioning Windows</t>
+  </si>
+  <si>
+    <t>Function Time</t>
+  </si>
+  <si>
+    <t>Random Variability Percentage</t>
+  </si>
+  <si>
+    <t>Function Cycle</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Fixed Cycle</t>
+  </si>
+  <si>
+    <t>Occasional Use</t>
+  </si>
+  <si>
+    <t>Flat</t>
+  </si>
+  <si>
+    <t>Thermal Power Variation</t>
+  </si>
+  <si>
+    <t>Preference Index</t>
+  </si>
+  <si>
+    <t>Weekday/Weekend Type</t>
+  </si>
+  <si>
+    <t>Year Minimum</t>
+  </si>
+  <si>
+    <t>Initial Share</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +142,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -196,10 +195,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -580,31 +579,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A03B1C-7874-4F43-9A9A-C3425B424BF6}">
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection sqref="A1:V4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="4" max="4" width="11.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.140625" style="1" customWidth="1"/>
     <col min="19" max="20" width="13" style="1" customWidth="1"/>
     <col min="21" max="21" width="12.140625" style="1" customWidth="1"/>
@@ -612,77 +611,68 @@
     <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:19" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="B2" s="1">
         <v>5</v>
@@ -691,10 +681,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="F2" s="1">
         <v>6</v>
@@ -716,9 +706,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>23</v>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -727,10 +717,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>22</v>
+        <v>4</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="F3" s="1">
         <v>3</v>
@@ -752,12 +742,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>22</v>
+        <v>5</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
@@ -776,11 +766,6 @@
         <v>0.1</v>
       </c>
       <c r="K4" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tester endring i kode
</commit_message>
<xml_diff>
--- a/Load_Profile/ramp/input_files/Appliances_and_users.xlsx
+++ b/Load_Profile/ramp/input_files/Appliances_and_users.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varsh\PycharmProjects\SizingOffGridMicrogrids\Load_Profile\ramp\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE80BB2-51EA-4527-9074-0056D5786C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3172E749-4E5C-432D-A023-05F8C0F061B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6165" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{DD404E9A-0D1E-45D4-8190-461235976194}"/>
+    <workbookView xWindow="4455" yWindow="600" windowWidth="13065" windowHeight="13515" activeTab="1" xr2:uid="{DD404E9A-0D1E-45D4-8190-461235976194}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" r:id="rId1"/>
-    <sheet name="Spring" sheetId="2" r:id="rId2"/>
-    <sheet name="Summer" sheetId="3" r:id="rId3"/>
-    <sheet name="Autumn" sheetId="4" r:id="rId4"/>
-    <sheet name="Winter" sheetId="5" r:id="rId5"/>
+    <sheet name="Appliances" sheetId="6" r:id="rId2"/>
+    <sheet name="Spring" sheetId="2" r:id="rId3"/>
+    <sheet name="Summer" sheetId="3" r:id="rId4"/>
+    <sheet name="Autumn" sheetId="4" r:id="rId5"/>
+    <sheet name="Winter" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>A</t>
   </si>
@@ -115,13 +116,79 @@
   </si>
   <si>
     <t>Initial Share</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>n_users</t>
+  </si>
+  <si>
+    <t>us_pref</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>num_windows</t>
+  </si>
+  <si>
+    <t>func_time</t>
+  </si>
+  <si>
+    <t>r_t</t>
+  </si>
+  <si>
+    <t>func_cycle</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>fixed_cycle</t>
+  </si>
+  <si>
+    <t>occasional_use</t>
+  </si>
+  <si>
+    <t>flat</t>
+  </si>
+  <si>
+    <t>thermal_P_var</t>
+  </si>
+  <si>
+    <t>pref_index</t>
+  </si>
+  <si>
+    <t>wd_we_type</t>
+  </si>
+  <si>
+    <t>year_min</t>
+  </si>
+  <si>
+    <t>initial_share</t>
+  </si>
+  <si>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>User2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,16 +218,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.6"/>
+      <color rgb="FFD1D5DB"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color rgb="FFD1D5DB"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF444654"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -177,11 +262,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD9D9E3"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFD9D9E3"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD9D9E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD9D9E3"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD9D9E3"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD9D9E3"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD9D9E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD9D9E3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD9D9E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD9D9E3"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD9D9E3"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD9D9E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -197,6 +334,19 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -575,11 +725,320 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FA8317-AF85-451D-8F1B-FDF9620D9149}">
+  <dimension ref="A1:S5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="6"/>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="9">
+        <v>10</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9">
+        <v>100</v>
+      </c>
+      <c r="G2" s="9">
+        <v>2</v>
+      </c>
+      <c r="H2" s="9">
+        <v>60</v>
+      </c>
+      <c r="I2" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="J2" s="9">
+        <v>30</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="9">
+        <v>1</v>
+      </c>
+      <c r="M2" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="P2" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>0</v>
+      </c>
+      <c r="R2" s="9">
+        <v>2020</v>
+      </c>
+      <c r="S2" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="9">
+        <v>10</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9">
+        <v>200</v>
+      </c>
+      <c r="G3" s="9">
+        <v>3</v>
+      </c>
+      <c r="H3" s="9">
+        <v>120</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="J3" s="9">
+        <v>60</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="9">
+        <v>2</v>
+      </c>
+      <c r="M3" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="P3" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>1</v>
+      </c>
+      <c r="R3" s="9">
+        <v>2021</v>
+      </c>
+      <c r="S3" s="10">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="9">
+        <v>20</v>
+      </c>
+      <c r="D4" s="9">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9">
+        <v>300</v>
+      </c>
+      <c r="G4" s="9">
+        <v>2</v>
+      </c>
+      <c r="H4" s="9">
+        <v>60</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="J4" s="9">
+        <v>30</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="9">
+        <v>1</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="P4" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>0</v>
+      </c>
+      <c r="R4" s="9">
+        <v>2020</v>
+      </c>
+      <c r="S4" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="9">
+        <v>20</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2</v>
+      </c>
+      <c r="E5" s="9">
+        <v>2</v>
+      </c>
+      <c r="F5" s="9">
+        <v>400</v>
+      </c>
+      <c r="G5" s="9">
+        <v>3</v>
+      </c>
+      <c r="H5" s="9">
+        <v>120</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="J5" s="9">
+        <v>60</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="9">
+        <v>2</v>
+      </c>
+      <c r="M5" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="P5" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>1</v>
+      </c>
+      <c r="R5" s="9">
+        <v>2021</v>
+      </c>
+      <c r="S5" s="10">
+        <v>0.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A03B1C-7874-4F43-9A9A-C3425B424BF6}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="S50" sqref="S50"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30:P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,7 +1207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61575C7D-FBDA-4E67-9E33-CB8A07069642}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -760,7 +1219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97B9A23-9CEB-4761-BC4E-311C6B8DA4BD}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -778,7 +1237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8E4124C-D8C4-48E1-8BB2-D99A82487179}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
RAMP med excel som fungerer!
</commit_message>
<xml_diff>
--- a/Load_Profile/ramp/input_files/Appliances_and_users.xlsx
+++ b/Load_Profile/ramp/input_files/Appliances_and_users.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varsh\PycharmProjects\SizingOffGridMicrogrids\Load_Profile\ramp\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3172E749-4E5C-432D-A023-05F8C0F061B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F1A85F-EA85-40FC-B8B4-1B8CEB2798B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="600" windowWidth="13065" windowHeight="13515" activeTab="1" xr2:uid="{DD404E9A-0D1E-45D4-8190-461235976194}"/>
+    <workbookView xWindow="-28920" yWindow="90" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{DD404E9A-0D1E-45D4-8190-461235976194}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" r:id="rId1"/>
-    <sheet name="Appliances" sheetId="6" r:id="rId2"/>
-    <sheet name="Spring" sheetId="2" r:id="rId3"/>
-    <sheet name="Summer" sheetId="3" r:id="rId4"/>
-    <sheet name="Autumn" sheetId="4" r:id="rId5"/>
-    <sheet name="Winter" sheetId="5" r:id="rId6"/>
+    <sheet name="User" sheetId="7" r:id="rId2"/>
+    <sheet name="Appliances_Spring" sheetId="6" r:id="rId3"/>
+    <sheet name="Spring" sheetId="2" r:id="rId4"/>
+    <sheet name="Summer" sheetId="3" r:id="rId5"/>
+    <sheet name="Autumn" sheetId="4" r:id="rId6"/>
+    <sheet name="Winter" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>A</t>
   </si>
@@ -172,23 +173,44 @@
     <t>initial_share</t>
   </si>
   <si>
-    <t>User1</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>User2</t>
+    <t>appliance_name</t>
+  </si>
+  <si>
+    <t>tele</t>
+  </si>
+  <si>
+    <t>soverom</t>
+  </si>
+  <si>
+    <t>stue</t>
+  </si>
+  <si>
+    <t>tv</t>
+  </si>
+  <si>
+    <t>seng</t>
+  </si>
+  <si>
+    <t>From_time</t>
+  </si>
+  <si>
+    <t>To_time</t>
+  </si>
+  <si>
+    <t>r_w</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,29 +242,29 @@
     </font>
     <font>
       <sz val="9.6"/>
-      <color rgb="FFD1D5DB"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="9.6"/>
-      <color rgb="FFD1D5DB"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF444654"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -318,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -335,19 +357,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,7 +746,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,307 +757,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FA8317-AF85-451D-8F1B-FDF9620D9149}">
-  <dimension ref="A1:S5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080047D7-4249-47B2-9B0B-B6BD385D918A}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="S1" s="6"/>
-    </row>
-    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>43</v>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
       </c>
       <c r="C2" s="9">
         <v>10</v>
       </c>
-      <c r="D2" s="9">
-        <v>1</v>
-      </c>
-      <c r="E2" s="9">
-        <v>1</v>
-      </c>
-      <c r="F2" s="9">
-        <v>100</v>
-      </c>
-      <c r="G2" s="9">
-        <v>2</v>
-      </c>
-      <c r="H2" s="9">
-        <v>60</v>
-      </c>
-      <c r="I2" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="J2" s="9">
-        <v>30</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="9">
-        <v>1</v>
-      </c>
-      <c r="M2" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="P2" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="9">
-        <v>0</v>
-      </c>
-      <c r="R2" s="9">
-        <v>2020</v>
-      </c>
-      <c r="S2" s="10">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>43</v>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
       </c>
       <c r="C3" s="9">
         <v>10</v>
       </c>
-      <c r="D3" s="9">
-        <v>1</v>
-      </c>
-      <c r="E3" s="9">
-        <v>2</v>
-      </c>
-      <c r="F3" s="9">
-        <v>200</v>
-      </c>
-      <c r="G3" s="9">
-        <v>3</v>
-      </c>
-      <c r="H3" s="9">
-        <v>120</v>
-      </c>
-      <c r="I3" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="J3" s="9">
-        <v>60</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="9">
-        <v>2</v>
-      </c>
-      <c r="M3" s="9">
-        <v>0.6</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="P3" s="9">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="9">
-        <v>1</v>
-      </c>
-      <c r="R3" s="9">
-        <v>2021</v>
-      </c>
-      <c r="S3" s="10">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
-        <v>2</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="9">
-        <v>20</v>
-      </c>
-      <c r="D4" s="9">
-        <v>2</v>
-      </c>
-      <c r="E4" s="9">
-        <v>1</v>
-      </c>
-      <c r="F4" s="9">
-        <v>300</v>
-      </c>
-      <c r="G4" s="9">
-        <v>2</v>
-      </c>
-      <c r="H4" s="9">
-        <v>60</v>
-      </c>
-      <c r="I4" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="J4" s="9">
-        <v>30</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" s="9">
-        <v>1</v>
-      </c>
-      <c r="M4" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="O4" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="P4" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="9">
-        <v>0</v>
-      </c>
-      <c r="R4" s="9">
-        <v>2020</v>
-      </c>
-      <c r="S4" s="10">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
-        <v>3</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="9">
-        <v>20</v>
-      </c>
-      <c r="D5" s="9">
-        <v>2</v>
-      </c>
-      <c r="E5" s="9">
-        <v>2</v>
-      </c>
-      <c r="F5" s="9">
-        <v>400</v>
-      </c>
-      <c r="G5" s="9">
-        <v>3</v>
-      </c>
-      <c r="H5" s="9">
-        <v>120</v>
-      </c>
-      <c r="I5" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="J5" s="9">
-        <v>60</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="9">
-        <v>2</v>
-      </c>
-      <c r="M5" s="9">
-        <v>0.6</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="O5" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="P5" s="9">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="9">
-        <v>1</v>
-      </c>
-      <c r="R5" s="9">
-        <v>2021</v>
-      </c>
-      <c r="S5" s="10">
-        <v>0.6</v>
-      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1034,6 +816,535 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FA8317-AF85-451D-8F1B-FDF9620D9149}">
+  <dimension ref="A1:T18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" customWidth="1"/>
+    <col min="15" max="15" width="20.5703125" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="16" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="6">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6">
+        <v>500</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6">
+        <f>3*60</f>
+        <v>180</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="6">
+        <v>5</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="N2" s="6">
+        <v>1</v>
+      </c>
+      <c r="O2" s="6">
+        <v>1</v>
+      </c>
+      <c r="P2" s="6">
+        <v>2020</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>0</v>
+      </c>
+      <c r="R2" s="10">
+        <f>7*60</f>
+        <v>420</v>
+      </c>
+      <c r="S2" s="10">
+        <f>17*60</f>
+        <v>1020</v>
+      </c>
+      <c r="T2" s="10">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="6">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6">
+        <v>400</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
+        <f t="shared" ref="F3:F5" si="0">3*60</f>
+        <v>180</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>5</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="6">
+        <v>1</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="N3" s="6">
+        <v>2</v>
+      </c>
+      <c r="O3" s="6">
+        <v>2</v>
+      </c>
+      <c r="P3" s="6">
+        <v>2021</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>0</v>
+      </c>
+      <c r="R3" s="10">
+        <f t="shared" ref="R3:R5" si="1">7*60</f>
+        <v>420</v>
+      </c>
+      <c r="S3" s="10">
+        <f t="shared" ref="S3:S5" si="2">17*60</f>
+        <v>1020</v>
+      </c>
+      <c r="T3" s="10">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="6">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6">
+        <v>700</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="6">
+        <v>5</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="N4" s="6">
+        <v>1</v>
+      </c>
+      <c r="O4" s="6">
+        <v>1</v>
+      </c>
+      <c r="P4" s="6">
+        <v>2020</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>0</v>
+      </c>
+      <c r="R4" s="10">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+      <c r="S4" s="10">
+        <f t="shared" si="2"/>
+        <v>1020</v>
+      </c>
+      <c r="T4" s="10">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="6">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6">
+        <v>50</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="6">
+        <v>5</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="6">
+        <v>1</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="N5" s="6">
+        <v>2</v>
+      </c>
+      <c r="O5" s="6">
+        <v>2</v>
+      </c>
+      <c r="P5" s="6">
+        <v>2021</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>0</v>
+      </c>
+      <c r="R5" s="10">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+      <c r="S5" s="10">
+        <f t="shared" si="2"/>
+        <v>1020</v>
+      </c>
+      <c r="T5" s="10">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="16"/>
+    </row>
+    <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
+      <c r="B15" s="11"/>
+    </row>
+    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="12"/>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A03B1C-7874-4F43-9A9A-C3425B424BF6}">
   <dimension ref="A1:S4"/>
   <sheetViews>
@@ -1207,7 +1518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61575C7D-FBDA-4E67-9E33-CB8A07069642}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1219,7 +1530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97B9A23-9CEB-4761-BC4E-311C6B8DA4BD}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1237,7 +1548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8E4124C-D8C4-48E1-8BB2-D99A82487179}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>